<commit_message>
Published state of ETDataset on 17 November 2017
</commit_message>
<xml_diff>
--- a/source_analyses/nl/2015/6_residences/6_residences_source_analysis_2015.xlsx
+++ b/source_analyses/nl/2015/6_residences/6_residences_source_analysis_2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53740" yWindow="-12500" windowWidth="24940" windowHeight="28340" tabRatio="710" activeTab="3"/>
+    <workbookView xWindow="53560" yWindow="-19540" windowWidth="24760" windowHeight="28340" tabRatio="710" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="4" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="249">
   <si>
     <t>Final demand per energy carrier</t>
   </si>
@@ -660,9 +660,6 @@
     <t>From ETSource</t>
   </si>
   <si>
-    <t>https://refman.energytransitionmodel.com/publications/2069</t>
-  </si>
-  <si>
     <t>hybrid heat pump (space heating</t>
   </si>
   <si>
@@ -840,30 +837,6 @@
     <t>Alternative calculation starting with gas use per household</t>
   </si>
   <si>
-    <t>HHP space</t>
-  </si>
-  <si>
-    <t>ambient</t>
-  </si>
-  <si>
-    <t>network gas</t>
-  </si>
-  <si>
-    <t>useable_heat</t>
-  </si>
-  <si>
-    <t>useable heat</t>
-  </si>
-  <si>
-    <t>HHP water</t>
-  </si>
-  <si>
-    <t>Heat output share</t>
-  </si>
-  <si>
-    <t>Carrier input share</t>
-  </si>
-  <si>
     <t>HHP for space heating</t>
   </si>
   <si>
@@ -871,33 +844,28 @@
   </si>
   <si>
     <t>FD share</t>
+  </si>
+  <si>
+    <t>Final demand share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="20">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="185" formatCode="#,##0.00000000000000000"/>
-    <numFmt numFmtId="186" formatCode="#,##0.000000000000000000"/>
-    <numFmt numFmtId="187" formatCode="#,##0.0000000000000000000"/>
-    <numFmt numFmtId="192" formatCode="#,##0.000000000000000000000000"/>
-    <numFmt numFmtId="196" formatCode="0.0000000000"/>
-    <numFmt numFmtId="199" formatCode="0.0000000000000"/>
-    <numFmt numFmtId="202" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="205" formatCode="0.0000000000000000000"/>
-    <numFmt numFmtId="206" formatCode="0.00000000000000000000"/>
-    <numFmt numFmtId="228" formatCode="0.000000000000000000000%"/>
-    <numFmt numFmtId="229" formatCode="0.0000000000000000000000%"/>
-    <numFmt numFmtId="235" formatCode="0.00000000000000000000000000000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00000000000000000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.0000000000000000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="174" formatCode="0.00000000000000000000000000000"/>
+    <numFmt numFmtId="175" formatCode="0.000%"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1903,7 +1871,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1943,7 +1910,6 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1962,8 +1928,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1978,7 +1942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1999,7 +1963,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2012,12 +1976,45 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2055,35 +2052,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="16" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="192" fontId="16" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="192" fontId="16" fillId="4" borderId="4" xfId="13" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="192" fontId="16" fillId="4" borderId="5" xfId="13" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="196" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="202" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="205" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="206" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="229" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="185" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="187" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="228" fontId="16" fillId="4" borderId="20" xfId="13" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="229" fontId="16" fillId="4" borderId="0" xfId="13" applyNumberFormat="1"/>
-    <xf numFmtId="229" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="235" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="205" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="199" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -2399,16 +2377,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>321733</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>135466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>385945</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>606206</xdr:rowOff>
+      <xdr:rowOff>403906</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2446,7 +2424,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>4538133</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>171824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3589,56 +3567,56 @@
       <c r="D29" s="111"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="264" t="s">
+      <c r="B30" s="279" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="265"/>
-      <c r="D30" s="266"/>
+      <c r="C30" s="280"/>
+      <c r="D30" s="281"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="264"/>
-      <c r="C31" s="265"/>
-      <c r="D31" s="266"/>
+      <c r="B31" s="279"/>
+      <c r="C31" s="280"/>
+      <c r="D31" s="281"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="264"/>
-      <c r="C32" s="265"/>
-      <c r="D32" s="266"/>
+      <c r="B32" s="279"/>
+      <c r="C32" s="280"/>
+      <c r="D32" s="281"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="264"/>
-      <c r="C33" s="265"/>
-      <c r="D33" s="266"/>
+      <c r="B33" s="279"/>
+      <c r="C33" s="280"/>
+      <c r="D33" s="281"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="264"/>
-      <c r="C34" s="265"/>
-      <c r="D34" s="266"/>
+      <c r="B34" s="279"/>
+      <c r="C34" s="280"/>
+      <c r="D34" s="281"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="264"/>
-      <c r="C35" s="265"/>
-      <c r="D35" s="266"/>
+      <c r="B35" s="279"/>
+      <c r="C35" s="280"/>
+      <c r="D35" s="281"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="264"/>
-      <c r="C36" s="265"/>
-      <c r="D36" s="266"/>
+      <c r="B36" s="279"/>
+      <c r="C36" s="280"/>
+      <c r="D36" s="281"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="264"/>
-      <c r="C37" s="265"/>
-      <c r="D37" s="266"/>
+      <c r="B37" s="279"/>
+      <c r="C37" s="280"/>
+      <c r="D37" s="281"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="264"/>
-      <c r="C38" s="265"/>
-      <c r="D38" s="266"/>
+      <c r="B38" s="279"/>
+      <c r="C38" s="280"/>
+      <c r="D38" s="281"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="267"/>
-      <c r="C39" s="268"/>
-      <c r="D39" s="269"/>
+      <c r="B39" s="282"/>
+      <c r="C39" s="283"/>
+      <c r="D39" s="284"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4189,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -4237,7 +4215,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
@@ -4250,7 +4228,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
@@ -4266,7 +4244,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
@@ -4274,7 +4252,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
@@ -4301,10 +4279,10 @@
   <dimension ref="B2:Q81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M42" sqref="M42"/>
+      <selection pane="bottomRight" activeCell="O26" activeCellId="1" sqref="O17 O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4368,14 +4346,14 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="270" t="s">
+      <c r="B5" s="285" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="271"/>
-      <c r="D5" s="271"/>
-      <c r="E5" s="271"/>
-      <c r="F5" s="271"/>
-      <c r="G5" s="272"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
+      <c r="G5" s="287"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -4429,7 +4407,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="2:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" ht="48" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -4495,27 +4473,27 @@
         <v>13</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="192">
+      <c r="E11" s="191">
         <v>285206.03000000003</v>
       </c>
-      <c r="F11" s="192">
+      <c r="F11" s="191">
         <v>81669.899999999994</v>
       </c>
-      <c r="G11" s="192">
+      <c r="G11" s="191">
         <v>909.83</v>
       </c>
-      <c r="H11" s="193">
+      <c r="H11" s="192">
         <v>270.01</v>
       </c>
-      <c r="I11" s="192">
+      <c r="I11" s="191">
         <f>1011.99+257.99+198.18</f>
         <v>1468.16</v>
       </c>
-      <c r="J11" s="192">
+      <c r="J11" s="191">
         <f>18364.48+20.01</f>
         <v>18384.489999999998</v>
       </c>
-      <c r="K11" s="192">
+      <c r="K11" s="191">
         <v>12075.69</v>
       </c>
       <c r="L11" s="57"/>
@@ -4529,11 +4507,11 @@
       <c r="D12" s="25"/>
       <c r="E12" s="57">
         <f t="shared" ref="E12:K12" si="0">SUM(E15:E26)</f>
-        <v>224517.83907059737</v>
+        <v>224517.8390705974</v>
       </c>
       <c r="F12" s="57">
         <f t="shared" si="0"/>
-        <v>6533.5920000000006</v>
+        <v>6533.5919999999996</v>
       </c>
       <c r="G12" s="57">
         <f t="shared" si="0"/>
@@ -4598,16 +4576,16 @@
       <c r="B15" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="211" t="s">
+      <c r="C15" s="209" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="83">
         <f>SUM(E15:K15)/SUM($E$15:$K$26)</f>
-        <v>0.82097666212909781</v>
+        <v>0.82093090361982568</v>
       </c>
       <c r="E15" s="78">
         <f>((E11-E52)*'Applicance split'!G25)-SUM(E16:E26)</f>
-        <v>215077.03485636218</v>
+        <v>215065.04717760382</v>
       </c>
       <c r="F15" s="78"/>
       <c r="G15" s="78"/>
@@ -4619,21 +4597,21 @@
       <c r="M15" s="10">
         <v>1.0669999999999999</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="175">
         <f t="shared" ref="N15:N25" si="1">M15*SUM(E15:K15)</f>
-        <v>229487.19619173845</v>
+        <v>229474.40533850327</v>
       </c>
       <c r="O15" s="106">
         <f>N15/SUM($N$15:$N$26)</f>
-        <v>0.83980550320000424</v>
+        <v>0.83996744920218935</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="288">
+      <c r="B16" s="259">
         <f>SUM(E15:K26)</f>
         <v>261977.03878522859</v>
       </c>
-      <c r="C16" s="212" t="s">
+      <c r="C16" s="210" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="84">
@@ -4654,28 +4632,28 @@
       <c r="M16" s="10">
         <v>1</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="175">
         <f t="shared" si="1"/>
         <v>756.90814993954052</v>
       </c>
       <c r="O16" s="106">
         <f t="shared" ref="O16:O25" si="3">N16/SUM($N$15:$N$26)</f>
-        <v>2.7698958385681113E-3</v>
+        <v>2.7705844015467095E-3</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
-      <c r="C17" s="212" t="s">
+      <c r="C17" s="210" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="84">
         <f t="shared" si="2"/>
-        <v>1.4544043935838674E-3</v>
+        <v>1.1241466273552163E-3</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="75">
         <f>'Heat pumps'!J21</f>
-        <v>381.02055622732769</v>
+        <v>294.50060459492141</v>
       </c>
       <c r="G17" s="75"/>
       <c r="H17" s="75"/>
@@ -4686,25 +4664,25 @@
       <c r="M17" s="10">
         <v>4.8000000000000078</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="175">
         <f t="shared" si="1"/>
-        <v>1828.8986698911758</v>
+        <v>1413.602902055625</v>
       </c>
       <c r="O17" s="106">
         <f t="shared" si="3"/>
-        <v>6.6928316405352054E-3</v>
+        <v>5.1743479717179875E-3</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
-      <c r="C18" s="212" t="s">
+      <c r="C18" s="210" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="84">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E18" s="210">
+      <c r="E18" s="208">
         <v>0</v>
       </c>
       <c r="F18" s="75"/>
@@ -4717,7 +4695,7 @@
       <c r="M18" s="10">
         <v>0.88</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="175">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4728,7 +4706,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
-      <c r="C19" s="212" t="s">
+      <c r="C19" s="210" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="84">
@@ -4749,28 +4727,28 @@
       <c r="M19" s="10">
         <v>1</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="175">
         <f t="shared" si="1"/>
         <v>10046.039564691657</v>
       </c>
       <c r="O19" s="106">
         <f t="shared" si="3"/>
-        <v>3.6763355218929421E-2</v>
+        <v>3.6772494149361512E-2</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="17"/>
-      <c r="C20" s="212" t="s">
+      <c r="C20" s="210" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="84">
         <f t="shared" si="2"/>
-        <v>8.1834778971689515E-4</v>
+        <v>1.0587663494077343E-3</v>
       </c>
       <c r="E20" s="75"/>
       <c r="F20" s="75">
         <f>'Heat pumps'!J19</f>
-        <v>214.38833064646914</v>
+        <v>277.37247298328492</v>
       </c>
       <c r="G20" s="75"/>
       <c r="H20" s="75"/>
@@ -4781,18 +4759,18 @@
       <c r="M20" s="10">
         <v>4.5000000000000044</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="175">
         <f t="shared" si="1"/>
-        <v>964.74748790911212</v>
+        <v>1248.1761284247834</v>
       </c>
       <c r="O20" s="106">
         <f t="shared" si="3"/>
-        <v>3.5304812773411676E-3</v>
+        <v>4.5688202882646937E-3</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="17"/>
-      <c r="C21" s="212" t="s">
+      <c r="C21" s="210" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="84">
@@ -4813,28 +4791,28 @@
       <c r="M21" s="10">
         <v>0.82</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="175">
         <f t="shared" si="1"/>
         <v>15075.281799999997</v>
       </c>
       <c r="O21" s="106">
         <f t="shared" si="3"/>
-        <v>5.5167803816614999E-2</v>
+        <v>5.5181517872858472E-2</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
-      <c r="C22" s="212" t="s">
+      <c r="C22" s="210" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="84">
         <f t="shared" si="2"/>
-        <v>2.2516763609382245E-2</v>
+        <v>2.2562522118654473E-2</v>
       </c>
       <c r="E22" s="75"/>
       <c r="F22" s="75">
         <f>Electricity!E38-SUM(F15:F21,F23:F26)</f>
-        <v>5898.8750534129558</v>
+        <v>5910.8627321713211</v>
       </c>
       <c r="G22" s="75"/>
       <c r="H22" s="75"/>
@@ -4845,25 +4823,25 @@
       <c r="M22" s="10">
         <v>1</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="175">
         <f t="shared" si="1"/>
-        <v>5898.8750534129558</v>
+        <v>5910.8627321713211</v>
       </c>
       <c r="O22" s="106">
         <f>N22/SUM($N$15:$N$26)</f>
-        <v>2.1586858939208045E-2</v>
+        <v>2.163610483880473E-2</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
-      <c r="C23" s="212" t="s">
+      <c r="C23" s="210" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="84">
         <f t="shared" si="2"/>
         <v>3.5881007143172626E-2</v>
       </c>
-      <c r="E23" s="210">
+      <c r="E23" s="208">
         <v>9400</v>
       </c>
       <c r="F23" s="75"/>
@@ -4876,18 +4854,18 @@
       <c r="M23" s="10">
         <v>0.8</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="175">
         <f t="shared" si="1"/>
         <v>7520</v>
       </c>
       <c r="O23" s="106">
         <f t="shared" si="3"/>
-        <v>2.7519345257011704E-2</v>
+        <v>2.7526186237122E-2</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="17"/>
-      <c r="C24" s="212" t="s">
+      <c r="C24" s="210" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="84">
@@ -4908,18 +4886,18 @@
       <c r="M24" s="10">
         <v>0.85</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="175">
         <f t="shared" si="1"/>
         <v>1247.9360000000001</v>
       </c>
       <c r="O24" s="106">
         <f t="shared" si="3"/>
-        <v>4.5668060695018831E-3</v>
+        <v>4.5679413228735489E-3</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="17"/>
-      <c r="C25" s="212" t="s">
+      <c r="C25" s="210" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="84">
@@ -4940,31 +4918,31 @@
       <c r="M25" s="10">
         <v>0.8</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="175">
         <f t="shared" si="1"/>
         <v>216.00800000000001</v>
       </c>
       <c r="O25" s="106">
         <f t="shared" si="3"/>
-        <v>7.9047855455805643E-4</v>
+        <v>7.9067505807290555E-4</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="17"/>
-      <c r="C26" s="213" t="s">
-        <v>187</v>
-      </c>
-      <c r="D26" s="290">
+      <c r="C26" s="211" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="84">
         <f t="shared" si="2"/>
-        <v>3.057988376383212E-4</v>
-      </c>
-      <c r="E26" s="280">
+        <v>3.9563804417613304E-4</v>
+      </c>
+      <c r="E26" s="75">
         <f>'Heat pumps'!K18</f>
-        <v>40.80421423520491</v>
-      </c>
-      <c r="F26" s="279">
+        <v>52.791892993570187</v>
+      </c>
+      <c r="F26" s="75">
         <f>'Heat pumps'!J18</f>
-        <v>39.308059713247388</v>
+        <v>50.856190250472608</v>
       </c>
       <c r="G26" s="75"/>
       <c r="H26" s="75"/>
@@ -4972,23 +4950,23 @@
       <c r="J26" s="75"/>
       <c r="K26" s="81"/>
       <c r="L26" s="90"/>
-      <c r="M26" s="205">
-        <f>1/'Heat pumps'!G4</f>
+      <c r="M26" s="203">
+        <f>1/'Heat pumps'!F4</f>
         <v>2.8070962566756963</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="175">
         <f>Q26*SUM(E26)+F26*P26</f>
-        <v>220.42436529857665</v>
-      </c>
-      <c r="O26" s="287">
+        <v>285.1818059512658</v>
+      </c>
+      <c r="O26" s="106">
         <f>N26/SUM($N$15:$N$26)</f>
-        <v>8.0664018772728724E-4</v>
+        <v>1.0438786571879428E-3</v>
       </c>
       <c r="P26" s="3">
         <f>('Heat pumps'!E5+'Heat pumps'!E4)/'Heat pumps'!E5</f>
         <v>4.4999999999999938</v>
       </c>
-      <c r="Q26" s="216">
+      <c r="Q26" s="212">
         <v>1.0669999999999999</v>
       </c>
     </row>
@@ -5004,16 +4982,16 @@
       <c r="J27" s="32"/>
       <c r="K27" s="33"/>
       <c r="L27" s="89"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="107"/>
+      <c r="M27" s="203"/>
+      <c r="N27" s="175"/>
+      <c r="O27" s="263"/>
       <c r="P27" s="3">
         <f>F26*P26</f>
-        <v>176.88626870961301</v>
+        <v>228.85285612712642</v>
       </c>
       <c r="Q27" s="3">
         <f>Q26*SUM(E26)</f>
-        <v>43.53809658896364</v>
+        <v>56.328949824139386</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.2">
@@ -5028,9 +5006,9 @@
       <c r="J28" s="36"/>
       <c r="K28" s="37"/>
       <c r="L28" s="89"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="107"/>
+      <c r="M28" s="203"/>
+      <c r="N28" s="175"/>
+      <c r="O28" s="263"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
@@ -5046,9 +5024,9 @@
       <c r="J29" s="58"/>
       <c r="K29" s="59"/>
       <c r="L29" s="64"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="107"/>
+      <c r="M29" s="203"/>
+      <c r="N29" s="175"/>
+      <c r="O29" s="106"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="24" t="s">
@@ -5057,13 +5035,13 @@
       <c r="C30" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="291">
+      <c r="D30" s="76">
         <f>SUM(E30:K30)/SUM($E$30:$K$42)</f>
-        <v>0.84162152462098438</v>
+        <v>0.84156200379083401</v>
       </c>
       <c r="E30" s="86">
         <f>((E11-E52)*'Applicance split'!G24)-SUM(E31:E42)</f>
-        <v>43449.975993405889</v>
+        <v>43446.903141101757</v>
       </c>
       <c r="F30" s="75"/>
       <c r="G30" s="75"/>
@@ -5072,28 +5050,28 @@
       <c r="J30" s="75"/>
       <c r="K30" s="81"/>
       <c r="L30" s="90"/>
-      <c r="M30" s="295">
+      <c r="M30" s="203">
         <v>0.9</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="175">
         <f t="shared" ref="N30:N36" si="4">M30*SUM(E30:K30)</f>
-        <v>39104.9783940653</v>
-      </c>
-      <c r="O30" s="287">
+        <v>39102.212826991585</v>
+      </c>
+      <c r="O30" s="106">
         <f>N30/SUM($N$30:$N$42)</f>
-        <v>0.83722902080194772</v>
+        <v>0.83728273296636391</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="289">
+      <c r="B31" s="260">
         <f>SUM(E30:K42)</f>
         <v>51626.502795271474</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="291">
-        <f t="shared" ref="D30:D42" si="5">SUM(E31:K31)/SUM($E$30:$K$42)</f>
+      <c r="D31" s="76">
+        <f t="shared" ref="D31:D42" si="5">SUM(E31:K31)/SUM($E$30:$K$42)</f>
         <v>2.962080361454694E-3</v>
       </c>
       <c r="E31" s="74"/>
@@ -5107,16 +5085,16 @@
       <c r="J31" s="75"/>
       <c r="K31" s="81"/>
       <c r="L31" s="90"/>
-      <c r="M31" s="295">
+      <c r="M31" s="203">
         <v>1</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="175">
         <f t="shared" si="4"/>
         <v>152.92185006045949</v>
       </c>
-      <c r="O31" s="287">
+      <c r="O31" s="106">
         <f t="shared" ref="O31:O42" si="6">N31/SUM($N$30:$N$42)</f>
-        <v>3.2740233096451759E-3</v>
+        <v>3.2744649290157575E-3</v>
       </c>
     </row>
     <row r="32" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5124,14 +5102,14 @@
       <c r="C32" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="291">
+      <c r="D32" s="76">
         <f t="shared" si="5"/>
-        <v>1.4910838349430659E-3</v>
+        <v>1.1524971125979157E-3</v>
       </c>
       <c r="E32" s="74"/>
       <c r="F32" s="75">
         <f>'Heat pumps'!L21</f>
-        <v>76.979443772672298</v>
+        <v>59.499395405078594</v>
       </c>
       <c r="G32" s="75"/>
       <c r="H32" s="75"/>
@@ -5139,16 +5117,16 @@
       <c r="J32" s="75"/>
       <c r="K32" s="81"/>
       <c r="L32" s="90"/>
-      <c r="M32" s="295">
+      <c r="M32" s="203">
         <v>3.0000000000000031</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="175">
         <f t="shared" si="4"/>
-        <v>230.93833131801713</v>
-      </c>
-      <c r="O32" s="287">
+        <v>178.49818621523596</v>
+      </c>
+      <c r="O32" s="106">
         <f t="shared" si="6"/>
-        <v>4.9443390825236319E-3</v>
+        <v>3.8221225444475758E-3</v>
       </c>
     </row>
     <row r="33" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5156,11 +5134,11 @@
       <c r="C33" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="291">
+      <c r="D33" s="76">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E33" s="191">
+      <c r="E33" s="190">
         <v>0</v>
       </c>
       <c r="F33" s="75"/>
@@ -5170,14 +5148,14 @@
       <c r="J33" s="75"/>
       <c r="K33" s="81"/>
       <c r="L33" s="90"/>
-      <c r="M33" s="295">
+      <c r="M33" s="203">
         <v>0.88</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="175">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O33" s="287">
+      <c r="O33" s="106">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5187,7 +5165,7 @@
       <c r="C34" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="291">
+      <c r="D34" s="76">
         <f t="shared" si="5"/>
         <v>3.9314118241885659E-2</v>
       </c>
@@ -5202,16 +5180,16 @@
         <v>2029.6504353083433</v>
       </c>
       <c r="L34" s="90"/>
-      <c r="M34" s="295">
+      <c r="M34" s="203">
         <v>1</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N34" s="175">
         <f t="shared" si="4"/>
         <v>2029.6504353083433</v>
       </c>
-      <c r="O34" s="287">
+      <c r="O34" s="106">
         <f t="shared" si="6"/>
-        <v>4.3454371190276377E-2</v>
+        <v>4.3460232569453958E-2</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -5219,14 +5197,14 @@
       <c r="C35" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="291">
+      <c r="D35" s="76">
         <f t="shared" si="5"/>
-        <v>8.1483086462928993E-4</v>
+        <v>1.0542162033904371E-3</v>
       </c>
       <c r="E35" s="74"/>
       <c r="F35" s="75">
         <f>'Heat pumps'!L19</f>
-        <v>42.066867910457511</v>
+        <v>54.425495771156882</v>
       </c>
       <c r="G35" s="75"/>
       <c r="H35" s="75"/>
@@ -5234,16 +5212,16 @@
       <c r="J35" s="75"/>
       <c r="K35" s="81"/>
       <c r="L35" s="90"/>
-      <c r="M35" s="295">
+      <c r="M35" s="203">
         <v>3.0000000000000031</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N35" s="175">
         <f t="shared" si="4"/>
-        <v>126.20060373137267</v>
-      </c>
-      <c r="O35" s="287">
+        <v>163.27648731347082</v>
+      </c>
+      <c r="O35" s="106">
         <f t="shared" si="6"/>
-        <v>2.7019272794859004E-3</v>
+        <v>3.4961853471526072E-3</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
@@ -5251,7 +5229,7 @@
       <c r="C36" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="291">
+      <c r="D36" s="76">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -5263,14 +5241,14 @@
       <c r="J36" s="75"/>
       <c r="K36" s="81"/>
       <c r="L36" s="90"/>
-      <c r="M36" s="295">
+      <c r="M36" s="203">
         <v>0.82</v>
       </c>
-      <c r="N36" s="2">
+      <c r="N36" s="175">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O36" s="287">
+      <c r="O36" s="106">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5280,14 +5258,14 @@
       <c r="C37" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="291">
+      <c r="D37" s="76">
         <f t="shared" si="5"/>
-        <v>7.6655893059668787E-2</v>
+        <v>7.6715413889819187E-2</v>
       </c>
       <c r="E37" s="74"/>
       <c r="F37" s="75">
         <f>Electricity!E39-SUM(F30:F36,F38:F42)</f>
-        <v>3957.4756773190215</v>
+        <v>3960.5485296231582</v>
       </c>
       <c r="G37" s="75"/>
       <c r="H37" s="75"/>
@@ -5295,16 +5273,16 @@
       <c r="J37" s="75"/>
       <c r="K37" s="81"/>
       <c r="L37" s="90"/>
-      <c r="M37" s="295">
+      <c r="M37" s="203">
         <v>0.95</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N37" s="175">
         <f>M37*SUM(E37:K37)</f>
-        <v>3759.6018934530703</v>
-      </c>
-      <c r="O37" s="287">
+        <v>3762.5211031419999</v>
+      </c>
+      <c r="O37" s="106">
         <f t="shared" si="6"/>
-        <v>8.0492252933671488E-2</v>
+        <v>8.056561826873794E-2</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5312,11 +5290,11 @@
       <c r="C38" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="291">
+      <c r="D38" s="76">
         <f t="shared" si="5"/>
         <v>3.6802802768465329E-2</v>
       </c>
-      <c r="E38" s="209">
+      <c r="E38" s="207">
         <v>1900</v>
       </c>
       <c r="F38" s="75"/>
@@ -5326,25 +5304,25 @@
       <c r="J38" s="75"/>
       <c r="K38" s="81"/>
       <c r="L38" s="90"/>
-      <c r="M38" s="295">
+      <c r="M38" s="203">
         <v>0.67</v>
       </c>
-      <c r="N38" s="2">
+      <c r="N38" s="175">
         <f>M38*SUM(E38:K38)</f>
         <v>1273</v>
       </c>
-      <c r="O38" s="287">
+      <c r="O38" s="106">
         <f t="shared" si="6"/>
-        <v>2.7254651127556373E-2</v>
-      </c>
-      <c r="P38" s="208"/>
+        <v>2.7258327393953414E-2</v>
+      </c>
+      <c r="P38" s="206"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="17"/>
       <c r="C39" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="291">
+      <c r="D39" s="76">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -5358,14 +5336,14 @@
       <c r="J39" s="75"/>
       <c r="K39" s="81"/>
       <c r="L39" s="90"/>
-      <c r="M39" s="295">
+      <c r="M39" s="203">
         <v>0.85</v>
       </c>
-      <c r="N39" s="2">
+      <c r="N39" s="175">
         <f>M39*SUM(E39:K39)</f>
         <v>0</v>
       </c>
-      <c r="O39" s="287">
+      <c r="O39" s="106">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5375,7 +5353,7 @@
       <c r="C40" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="291">
+      <c r="D40" s="76">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -5389,14 +5367,14 @@
       <c r="J40" s="75"/>
       <c r="K40" s="81"/>
       <c r="L40" s="90"/>
-      <c r="M40" s="295">
+      <c r="M40" s="203">
         <v>0.8</v>
       </c>
-      <c r="N40" s="2">
+      <c r="N40" s="175">
         <f>M40*SUM(E40:K40)</f>
         <v>0</v>
       </c>
-      <c r="O40" s="287">
+      <c r="O40" s="106">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5406,7 +5384,7 @@
       <c r="C41" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="291">
+      <c r="D41" s="76">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -5420,34 +5398,34 @@
       <c r="J41" s="75"/>
       <c r="K41" s="81"/>
       <c r="L41" s="90"/>
-      <c r="M41" s="295">
+      <c r="M41" s="203">
         <v>0.2</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41" s="175">
         <f>Q42*SUM(E41)+F41*P42</f>
         <v>0</v>
       </c>
-      <c r="O41" s="287">
+      <c r="O41" s="106">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="17"/>
-      <c r="C42" s="213" t="s">
-        <v>204</v>
-      </c>
-      <c r="D42" s="291">
+      <c r="C42" s="211" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" s="76">
         <f t="shared" si="5"/>
-        <v>3.376662479686257E-4</v>
-      </c>
-      <c r="E42" s="281">
+        <v>4.3686763155262857E-4</v>
+      </c>
+      <c r="E42" s="79">
         <f>'Heat pumps'!M18</f>
-        <v>10.459516496772652</v>
-      </c>
-      <c r="F42" s="282">
+        <v>13.532368800909246</v>
+      </c>
+      <c r="F42" s="73">
         <f>'Heat pumps'!L18</f>
-        <v>6.9730109978484336</v>
+        <v>9.0215792006061637</v>
       </c>
       <c r="G42" s="73"/>
       <c r="H42" s="73"/>
@@ -5455,20 +5433,20 @@
       <c r="J42" s="73"/>
       <c r="K42" s="82"/>
       <c r="L42" s="90"/>
-      <c r="M42" s="295">
-        <f>1/'Heat pumps'!I4</f>
+      <c r="M42" s="203">
+        <f>1/'Heat pumps'!H4</f>
         <v>1.687500000000002</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N42" s="175">
         <f>Q42*SUM(E42)+F42*P42</f>
-        <v>30.33259784064072</v>
-      </c>
-      <c r="O42" s="287">
+        <v>39.243869522636857</v>
+      </c>
+      <c r="O42" s="106">
         <f t="shared" si="6"/>
-        <v>6.4941427489326989E-4</v>
+        <v>8.4031598087480413E-4</v>
       </c>
       <c r="P42" s="3">
-        <f>('Heat pumps'!H5+'Heat pumps'!H4)/'Heat pumps'!H5</f>
+        <f>('Heat pumps'!G5+'Heat pumps'!G4)/'Heat pumps'!G5</f>
         <v>3.0000000000000044</v>
       </c>
       <c r="Q42" s="3">
@@ -5478,9 +5456,9 @@
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="17"/>
       <c r="C43" s="30"/>
-      <c r="D43" s="292">
+      <c r="D43" s="70">
         <f>SUM(D41:D42)</f>
-        <v>3.376662479686257E-4</v>
+        <v>4.3686763155262857E-4</v>
       </c>
       <c r="E43" s="64"/>
       <c r="F43" s="64"/>
@@ -5491,15 +5469,15 @@
       <c r="K43" s="65"/>
       <c r="L43" s="64"/>
       <c r="M43" s="10"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="107"/>
+      <c r="N43" s="175"/>
+      <c r="O43" s="106"/>
       <c r="P43" s="3">
         <f>F42*P42</f>
-        <v>20.919032993545333</v>
+        <v>27.064737601818532</v>
       </c>
       <c r="Q43" s="3">
         <f>Q42*SUM(E42)</f>
-        <v>9.4135648470953868</v>
+        <v>12.179131920818323</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
@@ -5561,7 +5539,7 @@
       <c r="M46" s="10">
         <v>4.6000000000000023</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="175">
         <f>M46*SUM(E46:K46)</f>
         <v>2536.3888888888887</v>
       </c>
@@ -5595,7 +5573,7 @@
       <c r="M47" s="10">
         <v>4.5000000000000044</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N47" s="175">
         <f>M47*SUM(E47:K47)</f>
         <v>0</v>
       </c>
@@ -5627,7 +5605,7 @@
       <c r="M48" s="10">
         <v>4</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48" s="175">
         <f>M48*SUM(E48:K48)</f>
         <v>23928.812444444444</v>
       </c>
@@ -5649,7 +5627,7 @@
       <c r="K49" s="65"/>
       <c r="L49" s="64"/>
       <c r="M49" s="10"/>
-      <c r="N49" s="2"/>
+      <c r="N49" s="175"/>
       <c r="O49" s="107"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
@@ -5665,7 +5643,7 @@
       <c r="K50" s="59"/>
       <c r="L50" s="64"/>
       <c r="M50" s="10"/>
-      <c r="N50" s="2"/>
+      <c r="N50" s="175"/>
       <c r="O50" s="107"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
@@ -5683,7 +5661,7 @@
       <c r="K51" s="59"/>
       <c r="L51" s="64"/>
       <c r="M51" s="10"/>
-      <c r="N51" s="2"/>
+      <c r="N51" s="175"/>
       <c r="O51" s="107"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
@@ -5711,7 +5689,7 @@
       <c r="M52" s="10">
         <v>0.4</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N52" s="175">
         <f>M52*SUM(E52:K52)</f>
         <v>6131.1021677999997</v>
       </c>
@@ -5746,7 +5724,7 @@
       <c r="M53" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N53" s="175">
         <f>M53*SUM(E53:K53)</f>
         <v>262.31000324427475</v>
       </c>
@@ -5778,7 +5756,7 @@
       <c r="M54" s="10">
         <v>0.6</v>
       </c>
-      <c r="N54" s="2">
+      <c r="N54" s="175">
         <f>M54*SUM(E54:K54)</f>
         <v>2098.480025954198</v>
       </c>
@@ -5810,7 +5788,7 @@
       <c r="M55" s="10">
         <v>0.85</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="175">
         <f>M55*SUM(E55:K55)</f>
         <v>786.93000973282426</v>
       </c>
@@ -5841,7 +5819,7 @@
       <c r="M56" s="10">
         <v>0.3</v>
       </c>
-      <c r="N56" s="2">
+      <c r="N56" s="175">
         <f>M56*SUM(E56:K56)</f>
         <v>0</v>
       </c>
@@ -5863,7 +5841,7 @@
       <c r="K57" s="62"/>
       <c r="L57" s="64"/>
       <c r="M57" s="10"/>
-      <c r="N57" s="2"/>
+      <c r="N57" s="175"/>
       <c r="O57" s="107"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
@@ -5879,7 +5857,7 @@
       <c r="K58" s="59"/>
       <c r="L58" s="64"/>
       <c r="M58" s="10"/>
-      <c r="N58" s="2"/>
+      <c r="N58" s="175"/>
       <c r="O58" s="107"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
@@ -5897,7 +5875,7 @@
       <c r="K59" s="58"/>
       <c r="L59" s="91"/>
       <c r="M59" s="10"/>
-      <c r="N59" s="2"/>
+      <c r="N59" s="175"/>
       <c r="O59" s="107"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
@@ -5925,7 +5903,7 @@
       <c r="M60" s="10">
         <v>0.05</v>
       </c>
-      <c r="N60" s="173">
+      <c r="N60" s="264">
         <f>O60/M60</f>
         <v>9.8999999999999986</v>
       </c>
@@ -5962,7 +5940,7 @@
       <c r="M61" s="10">
         <v>0.25</v>
       </c>
-      <c r="N61" s="173">
+      <c r="N61" s="264">
         <f>O61/M61</f>
         <v>1.94</v>
       </c>
@@ -5996,7 +5974,7 @@
       <c r="M62" s="10">
         <v>0.5</v>
       </c>
-      <c r="N62" s="173">
+      <c r="N62" s="264">
         <f>O62/M62</f>
         <v>0.04</v>
       </c>
@@ -6496,17 +6474,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F24">
         <v>55.6</v>
@@ -6535,16 +6513,16 @@
       <c r="F26">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G26" s="174"/>
+      <c r="G26" s="173"/>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F27">
         <v>64.099999999999994</v>
       </c>
-      <c r="G27" s="174"/>
+      <c r="G27" s="173"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7053,567 +7031,567 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K7" s="219"/>
+      <c r="K7" s="215"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K8" s="219"/>
+      <c r="K8" s="215"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K9" s="219"/>
+      <c r="K9" s="215"/>
     </row>
     <row r="18" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="197" t="s">
+      <c r="B19" s="196" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="197" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="198" t="s">
+      <c r="D19" s="197" t="s">
         <v>238</v>
       </c>
-      <c r="D19" s="198" t="s">
+      <c r="E19" s="220" t="s">
         <v>239</v>
       </c>
-      <c r="E19" s="224" t="s">
+    </row>
+    <row r="20" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="223">
+        <v>530</v>
+      </c>
+      <c r="C20" s="224" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="224" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" s="225" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="227">
-        <v>530</v>
-      </c>
-      <c r="C20" s="228" t="s">
-        <v>215</v>
-      </c>
-      <c r="D20" s="228" t="s">
-        <v>232</v>
-      </c>
-      <c r="E20" s="229" t="s">
+    <row r="21" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="226">
+        <v>3.5999999999999998E-6</v>
+      </c>
+      <c r="C21" s="224" t="s">
+        <v>230</v>
+      </c>
+      <c r="D21" s="224"/>
+      <c r="E21" s="225" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="230">
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="C21" s="228" t="s">
-        <v>231</v>
-      </c>
-      <c r="D21" s="228"/>
-      <c r="E21" s="229" t="s">
-        <v>242</v>
-      </c>
-    </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="231">
+      <c r="B22" s="227">
         <f>B20*B21</f>
         <v>1.908E-3</v>
       </c>
-      <c r="C22" s="228" t="s">
+      <c r="C22" s="224" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="228" t="s">
-        <v>233</v>
-      </c>
-      <c r="E22" s="229"/>
+      <c r="D22" s="224" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" s="225"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="232">
+      <c r="B23" s="228">
         <f>SUMPRODUCT(C36:C38,D36:D38)/SUM(C36:C38)</f>
         <v>0.65833333333333333</v>
       </c>
-      <c r="C23" s="228" t="s">
+      <c r="C23" s="224" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="228" t="s">
-        <v>219</v>
-      </c>
-      <c r="E23" s="229"/>
+      <c r="D23" s="224" t="s">
+        <v>218</v>
+      </c>
+      <c r="E23" s="225"/>
     </row>
     <row r="24" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="231">
+      <c r="B24" s="227">
         <f>B22*B23</f>
         <v>1.2561E-3</v>
       </c>
-      <c r="C24" s="228" t="s">
+      <c r="C24" s="224" t="s">
         <v>162</v>
       </c>
-      <c r="D24" s="228" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" s="229"/>
+      <c r="D24" s="224" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="225"/>
     </row>
     <row r="25" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="233">
+      <c r="B25" s="229">
         <v>7449298</v>
       </c>
-      <c r="C25" s="228" t="s">
-        <v>222</v>
-      </c>
-      <c r="D25" s="228" t="s">
+      <c r="C25" s="224" t="s">
         <v>221</v>
       </c>
-      <c r="E25" s="229" t="s">
-        <v>243</v>
+      <c r="D25" s="224" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" s="225" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="231">
+      <c r="B26" s="227">
         <f>B24*B25</f>
         <v>9357.0632177999996</v>
       </c>
-      <c r="C26" s="228" t="s">
+      <c r="C26" s="224" t="s">
         <v>162</v>
       </c>
-      <c r="D26" s="228" t="s">
-        <v>230</v>
-      </c>
-      <c r="E26" s="229"/>
+      <c r="D26" s="224" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" s="225"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="231">
+      <c r="B27" s="227">
         <f>G36*B23</f>
         <v>3225.9610499999994</v>
       </c>
-      <c r="C27" s="228" t="s">
+      <c r="C27" s="224" t="s">
         <v>162</v>
       </c>
-      <c r="D27" s="228" t="s">
-        <v>223</v>
-      </c>
-      <c r="E27" s="229"/>
+      <c r="D27" s="224" t="s">
+        <v>222</v>
+      </c>
+      <c r="E27" s="225"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="231">
+      <c r="B28" s="227">
         <f>B26-B27</f>
         <v>6131.1021677999997</v>
       </c>
-      <c r="C28" s="228" t="s">
+      <c r="C28" s="224" t="s">
         <v>162</v>
       </c>
-      <c r="D28" s="228" t="s">
-        <v>224</v>
-      </c>
-      <c r="E28" s="229"/>
+      <c r="D28" s="224" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" s="225"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="231">
+      <c r="B29" s="227">
         <f>B28/B26</f>
         <v>0.65523786952051</v>
       </c>
-      <c r="C29" s="228" t="s">
-        <v>220</v>
-      </c>
-      <c r="D29" s="228" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" s="229"/>
+      <c r="C29" s="224" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="224" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="225"/>
     </row>
     <row r="30" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="234">
+      <c r="B30" s="230">
         <f>B28/D39</f>
         <v>15327.755419499999</v>
       </c>
-      <c r="C30" s="235"/>
-      <c r="D30" s="235" t="s">
-        <v>234</v>
-      </c>
-      <c r="E30" s="236"/>
+      <c r="C30" s="231"/>
+      <c r="D30" s="231" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="232"/>
     </row>
     <row r="34" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:12" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="197" t="s">
+      <c r="B35" s="196" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="194" t="s">
+      <c r="C35" s="193" t="s">
         <v>142</v>
       </c>
-      <c r="D35" s="178" t="s">
+      <c r="D35" s="177" t="s">
         <v>161</v>
       </c>
-      <c r="E35" s="178" t="s">
+      <c r="E35" s="177" t="s">
         <v>143</v>
       </c>
-      <c r="F35" s="178" t="s">
+      <c r="F35" s="177" t="s">
+        <v>205</v>
+      </c>
+      <c r="G35" s="177" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35" s="197" t="s">
         <v>206</v>
       </c>
-      <c r="G35" s="178" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" s="198" t="s">
+      <c r="I35" s="177" t="s">
         <v>207</v>
       </c>
-      <c r="I35" s="178" t="s">
-        <v>208</v>
-      </c>
-      <c r="J35" s="198" t="s">
-        <v>236</v>
-      </c>
-      <c r="K35" s="224" t="s">
+      <c r="J35" s="197" t="s">
         <v>235</v>
       </c>
+      <c r="K35" s="220" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="36" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="226" t="s">
+      <c r="B36" s="222" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="192">
+      <c r="C36" s="191">
         <v>0.02</v>
       </c>
-      <c r="D36" s="237">
+      <c r="D36" s="233">
         <f>'Final demand per energy carrier'!M53</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="E36" s="228">
+      <c r="E36" s="224">
         <f>C36/D36</f>
         <v>3.6363636363636362E-2</v>
       </c>
-      <c r="F36" s="228">
+      <c r="F36" s="224">
         <f>E36/SUM($E$36:$E$38)</f>
         <v>9.7328244274809142E-2</v>
       </c>
-      <c r="G36" s="238">
+      <c r="G36" s="234">
         <f>Electricity!E41</f>
         <v>4900.1939999999995</v>
       </c>
-      <c r="H36" s="239">
+      <c r="H36" s="235">
         <f>F36*$G$36</f>
         <v>476.92727862595405</v>
       </c>
-      <c r="I36" s="228"/>
-      <c r="J36" s="228">
+      <c r="I36" s="224"/>
+      <c r="J36" s="224">
         <f>H36*D36</f>
         <v>262.31000324427475</v>
       </c>
-      <c r="K36" s="240">
+      <c r="K36" s="236">
         <f>J36/(SUM(J$36:J$39))</f>
         <v>2.8269752065513517E-2</v>
       </c>
-      <c r="L36" s="206"/>
+      <c r="L36" s="204"/>
     </row>
     <row r="37" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="195" t="s">
+      <c r="B37" s="194" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="192">
+      <c r="C37" s="191">
         <v>0.16</v>
       </c>
-      <c r="D37" s="237">
+      <c r="D37" s="233">
         <f>'Final demand per energy carrier'!M54</f>
         <v>0.6</v>
       </c>
-      <c r="E37" s="228">
+      <c r="E37" s="224">
         <f>C37/D37</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="F37" s="228">
+      <c r="F37" s="224">
         <f>E37/SUM($E$36:$E$38)</f>
         <v>0.71374045801526709</v>
       </c>
-      <c r="G37" s="228"/>
-      <c r="H37" s="239">
+      <c r="G37" s="224"/>
+      <c r="H37" s="235">
         <f>F37*$G$36</f>
         <v>3497.4667099236635</v>
       </c>
-      <c r="I37" s="228"/>
-      <c r="J37" s="228">
+      <c r="I37" s="224"/>
+      <c r="J37" s="224">
         <f>H37*D37</f>
         <v>2098.480025954198</v>
       </c>
-      <c r="K37" s="240">
+      <c r="K37" s="236">
         <f>J37/(SUM(J$36:J$39))</f>
         <v>0.22615801652410814</v>
       </c>
-      <c r="L37" s="206"/>
+      <c r="L37" s="204"/>
     </row>
     <row r="38" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="195" t="s">
+      <c r="B38" s="194" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="192">
+      <c r="C38" s="191">
         <v>0.06</v>
       </c>
-      <c r="D38" s="237">
+      <c r="D38" s="233">
         <f>'Final demand per energy carrier'!M55</f>
         <v>0.85</v>
       </c>
-      <c r="E38" s="228">
+      <c r="E38" s="224">
         <f>C38/D38</f>
         <v>7.0588235294117646E-2</v>
       </c>
-      <c r="F38" s="228">
+      <c r="F38" s="224">
         <f>E38/SUM($E$36:$E$38)</f>
         <v>0.18893129770992365</v>
       </c>
-      <c r="G38" s="228"/>
-      <c r="H38" s="239">
+      <c r="G38" s="224"/>
+      <c r="H38" s="235">
         <f>F38*$G$36</f>
         <v>925.80001145038148</v>
       </c>
-      <c r="I38" s="228"/>
-      <c r="J38" s="228">
+      <c r="I38" s="224"/>
+      <c r="J38" s="224">
         <f>H38*D38</f>
         <v>786.93000973282426</v>
       </c>
-      <c r="K38" s="240">
+      <c r="K38" s="236">
         <f>J38/(SUM(J$36:J$39))</f>
         <v>8.4809256196540547E-2</v>
       </c>
-      <c r="L38" s="206"/>
+      <c r="L38" s="204"/>
     </row>
     <row r="39" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="225" t="s">
+      <c r="B39" s="221" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="235"/>
-      <c r="D39" s="241">
+      <c r="C39" s="231"/>
+      <c r="D39" s="237">
         <f>'Final demand per energy carrier'!M52</f>
         <v>0.4</v>
       </c>
-      <c r="E39" s="241">
+      <c r="E39" s="237">
         <f>C39/D39</f>
         <v>0</v>
       </c>
-      <c r="F39" s="235"/>
-      <c r="G39" s="235"/>
-      <c r="H39" s="235"/>
-      <c r="I39" s="241">
+      <c r="F39" s="231"/>
+      <c r="G39" s="231"/>
+      <c r="H39" s="231"/>
+      <c r="I39" s="237">
         <f>B30</f>
         <v>15327.755419499999</v>
       </c>
-      <c r="J39" s="235">
+      <c r="J39" s="231">
         <f>I39*D39</f>
         <v>6131.1021677999997</v>
       </c>
-      <c r="K39" s="242">
+      <c r="K39" s="238">
         <f>J39/(SUM(J$36:J$39))</f>
         <v>0.66076297521383787</v>
       </c>
-      <c r="L39" s="206"/>
+      <c r="L39" s="204"/>
     </row>
     <row r="41" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B42" s="273" t="s">
-        <v>245</v>
-      </c>
-      <c r="C42" s="274"/>
-      <c r="D42" s="274"/>
-      <c r="E42" s="275"/>
+      <c r="B42" s="288" t="s">
+        <v>244</v>
+      </c>
+      <c r="C42" s="289"/>
+      <c r="D42" s="289"/>
+      <c r="E42" s="290"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="243" t="s">
+      <c r="B43" s="239" t="s">
+        <v>236</v>
+      </c>
+      <c r="C43" s="240" t="s">
         <v>237</v>
       </c>
-      <c r="C43" s="244" t="s">
+      <c r="D43" s="240" t="s">
         <v>238</v>
       </c>
-      <c r="D43" s="244" t="s">
+      <c r="E43" s="241" t="s">
         <v>239</v>
       </c>
-      <c r="E43" s="245" t="s">
+    </row>
+    <row r="44" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="242">
+        <v>65</v>
+      </c>
+      <c r="C44" s="243" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" s="243" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="244" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="246">
-        <v>65</v>
-      </c>
-      <c r="C44" s="247" t="s">
-        <v>216</v>
-      </c>
-      <c r="D44" s="247" t="s">
-        <v>225</v>
-      </c>
-      <c r="E44" s="248" t="s">
-        <v>241</v>
-      </c>
-    </row>
     <row r="45" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="249">
+      <c r="B45" s="245">
         <f>31.65/10^6</f>
         <v>3.1649999999999997E-5</v>
       </c>
-      <c r="C45" s="247" t="s">
+      <c r="C45" s="243" t="s">
+        <v>225</v>
+      </c>
+      <c r="D45" s="243" t="s">
         <v>226</v>
       </c>
-      <c r="D45" s="247" t="s">
-        <v>227</v>
-      </c>
-      <c r="E45" s="248" t="s">
-        <v>244</v>
+      <c r="E45" s="244" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="250">
+      <c r="B46" s="246">
         <f>B44*B45</f>
         <v>2.0572499999999996E-3</v>
       </c>
-      <c r="C46" s="247" t="s">
+      <c r="C46" s="243" t="s">
         <v>162</v>
       </c>
-      <c r="D46" s="247" t="s">
-        <v>217</v>
-      </c>
-      <c r="E46" s="248"/>
+      <c r="D46" s="243" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" s="244"/>
     </row>
     <row r="47" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="250">
+      <c r="B47" s="246">
         <f>B46*D39</f>
         <v>8.2289999999999989E-4</v>
       </c>
-      <c r="C47" s="247" t="s">
+      <c r="C47" s="243" t="s">
         <v>162</v>
       </c>
-      <c r="D47" s="247" t="s">
-        <v>218</v>
-      </c>
-      <c r="E47" s="248"/>
+      <c r="D47" s="243" t="s">
+        <v>217</v>
+      </c>
+      <c r="E47" s="244"/>
     </row>
     <row r="48" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="251">
+      <c r="B48" s="247">
         <v>7449298</v>
       </c>
-      <c r="C48" s="247" t="s">
-        <v>222</v>
-      </c>
-      <c r="D48" s="247" t="s">
+      <c r="C48" s="243" t="s">
         <v>221</v>
       </c>
-      <c r="E48" s="248" t="s">
-        <v>243</v>
+      <c r="D48" s="243" t="s">
+        <v>220</v>
+      </c>
+      <c r="E48" s="244" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="250">
+      <c r="B49" s="246">
         <f>B47*B48</f>
         <v>6130.0273241999994</v>
       </c>
-      <c r="C49" s="247" t="s">
+      <c r="C49" s="243" t="s">
         <v>162</v>
       </c>
-      <c r="D49" s="247" t="s">
-        <v>230</v>
-      </c>
-      <c r="E49" s="248"/>
+      <c r="D49" s="243" t="s">
+        <v>229</v>
+      </c>
+      <c r="E49" s="244"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="250">
+      <c r="B50" s="246">
         <f>SUMPRODUCT(C36:C38,D36:D38)/SUM(C36:C38)</f>
         <v>0.65833333333333333</v>
       </c>
-      <c r="C50" s="247" t="s">
-        <v>220</v>
-      </c>
-      <c r="D50" s="247" t="s">
+      <c r="C50" s="243" t="s">
         <v>219</v>
       </c>
-      <c r="E50" s="248"/>
+      <c r="D50" s="243" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50" s="244"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="250">
+      <c r="B51" s="246">
         <f>G36*B50</f>
         <v>3225.9610499999994</v>
       </c>
-      <c r="C51" s="247" t="s">
+      <c r="C51" s="243" t="s">
         <v>162</v>
       </c>
-      <c r="D51" s="247" t="s">
-        <v>223</v>
-      </c>
-      <c r="E51" s="252"/>
+      <c r="D51" s="243" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="248"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="250">
+      <c r="B52" s="246">
         <f>B49-B51</f>
         <v>2904.0662742</v>
       </c>
-      <c r="C52" s="247" t="s">
+      <c r="C52" s="243" t="s">
         <v>162</v>
       </c>
-      <c r="D52" s="247" t="s">
-        <v>224</v>
-      </c>
-      <c r="E52" s="253"/>
+      <c r="D52" s="243" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" s="249"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="250">
+      <c r="B53" s="246">
         <f>B52/D39</f>
         <v>7260.1656854999992</v>
       </c>
-      <c r="C53" s="247"/>
-      <c r="D53" s="247" t="s">
-        <v>229</v>
-      </c>
-      <c r="E53" s="252"/>
+      <c r="C53" s="243"/>
+      <c r="D53" s="243" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53" s="248"/>
     </row>
     <row r="54" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="254">
+      <c r="B54" s="250">
         <f>B52/B49</f>
         <v>0.47374442569536113</v>
       </c>
-      <c r="C54" s="255" t="s">
-        <v>220</v>
-      </c>
-      <c r="D54" s="255" t="s">
-        <v>228</v>
-      </c>
-      <c r="E54" s="256"/>
+      <c r="C54" s="251" t="s">
+        <v>219</v>
+      </c>
+      <c r="D54" s="251" t="s">
+        <v>227</v>
+      </c>
+      <c r="E54" s="252"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D62" s="220"/>
-      <c r="E62" s="207"/>
-      <c r="G62" s="218"/>
+      <c r="D62" s="216"/>
+      <c r="E62" s="205"/>
+      <c r="G62" s="214"/>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D63" s="220"/>
-      <c r="E63" s="207"/>
-      <c r="F63" s="218"/>
-      <c r="G63" s="218"/>
+      <c r="D63" s="216"/>
+      <c r="E63" s="205"/>
+      <c r="F63" s="214"/>
+      <c r="G63" s="214"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F64" s="218"/>
-      <c r="G64" s="218"/>
+      <c r="F64" s="214"/>
+      <c r="G64" s="214"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D65" s="221"/>
-      <c r="E65" s="207"/>
-      <c r="G65" s="218"/>
+      <c r="D65" s="217"/>
+      <c r="E65" s="205"/>
+      <c r="G65" s="214"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D66" s="221"/>
-      <c r="E66" s="207"/>
-      <c r="F66" s="218"/>
-      <c r="G66" s="218"/>
+      <c r="D66" s="217"/>
+      <c r="E66" s="205"/>
+      <c r="F66" s="214"/>
+      <c r="G66" s="214"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F67" s="218"/>
-      <c r="G67" s="218"/>
+      <c r="F67" s="214"/>
+      <c r="G67" s="214"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C69" s="218"/>
-      <c r="D69" s="221"/>
-      <c r="E69" s="207"/>
-      <c r="G69" s="222"/>
+      <c r="C69" s="214"/>
+      <c r="D69" s="217"/>
+      <c r="E69" s="205"/>
+      <c r="G69" s="218"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C70" s="223"/>
-      <c r="D70" s="221"/>
-      <c r="E70" s="207"/>
-      <c r="F70" s="222"/>
-      <c r="G70" s="218"/>
+      <c r="C70" s="219"/>
+      <c r="D70" s="217"/>
+      <c r="E70" s="205"/>
+      <c r="F70" s="218"/>
+      <c r="G70" s="214"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F71" s="218"/>
-      <c r="G71" s="218"/>
+      <c r="F71" s="214"/>
+      <c r="G71" s="214"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D72" s="221"/>
-      <c r="E72" s="207"/>
-      <c r="G72" s="218"/>
+      <c r="D72" s="217"/>
+      <c r="E72" s="205"/>
+      <c r="G72" s="214"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D73" s="221"/>
-      <c r="E73" s="207"/>
-      <c r="F73" s="218"/>
-      <c r="G73" s="218"/>
+      <c r="D73" s="217"/>
+      <c r="E73" s="205"/>
+      <c r="F73" s="214"/>
+      <c r="G73" s="214"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7632,10 +7610,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:O46"/>
+  <dimension ref="C1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScale="123" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="B1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7643,12 +7621,12 @@
     <col min="1" max="1" width="3.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="36" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="22" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -7657,334 +7635,322 @@
     <col min="16" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="276" t="s">
+    <row r="1" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="291" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="277"/>
-      <c r="E2" s="277"/>
-      <c r="F2" s="277"/>
-      <c r="G2" s="277"/>
-      <c r="H2" s="277"/>
-      <c r="I2" s="278"/>
-    </row>
-    <row r="3" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="10"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="2" t="s">
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292"/>
+      <c r="H2" s="293"/>
+    </row>
+    <row r="3" spans="3:14" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="268"/>
+      <c r="D3" s="274"/>
+      <c r="E3" s="276" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="277" t="s">
         <v>178</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="G3" s="276" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="278" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="175" t="s">
+      <c r="D4" s="174" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="257">
+      <c r="E4" s="253">
         <v>0.63199000312402398</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176">
+      <c r="F4" s="175">
         <f>SUM(E5,E6/E7)</f>
         <v>0.35624001051686416</v>
       </c>
-      <c r="H4" s="294">
+      <c r="G4" s="187">
         <v>0.44444444444444497</v>
       </c>
-      <c r="I4" s="177">
-        <f>SUM(H5,H6/H7)</f>
+      <c r="H4" s="176">
+        <f>SUM(G5,G6/G7)</f>
         <v>0.59259259259259189</v>
       </c>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-    </row>
-    <row r="5" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="175"/>
+      <c r="J4" s="175"/>
+    </row>
+    <row r="5" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="174" t="s">
         <v>180</v>
       </c>
-      <c r="E5" s="257">
+      <c r="E5" s="253">
         <v>0.18056857232115001</v>
       </c>
-      <c r="F5" s="176"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="294">
+      <c r="F5" s="2"/>
+      <c r="G5" s="187">
         <v>0.22222222222222199</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="O5" s="186" t="s">
+      <c r="H5" s="11"/>
+      <c r="N5" s="185" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="10"/>
-      <c r="D6" s="175" t="s">
+      <c r="D6" s="174" t="s">
         <v>181</v>
       </c>
-      <c r="E6" s="257">
+      <c r="E6" s="253">
         <v>0.18744142455482701</v>
       </c>
-      <c r="F6" s="176"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="294">
+      <c r="F6" s="2"/>
+      <c r="G6" s="187">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="3:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="10"/>
-      <c r="D7" s="175" t="s">
-        <v>209</v>
-      </c>
-      <c r="E7" s="263">
+      <c r="D7" s="275" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="257">
         <v>1.0669999999999999</v>
       </c>
-      <c r="F7" s="176"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="187">
+      <c r="F7" s="2"/>
+      <c r="G7" s="187">
         <v>0.9</v>
       </c>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
-      <c r="D8" s="175"/>
-      <c r="E8" s="176"/>
-      <c r="F8" s="176"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="174"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="175"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="175" t="s">
+      <c r="D9" s="174" t="s">
         <v>182</v>
       </c>
-      <c r="E9" s="188">
+      <c r="E9" s="187">
         <v>0.77777777777777801</v>
       </c>
-      <c r="F9" s="176"/>
-      <c r="G9" s="176">
+      <c r="F9" s="175">
         <f>E10</f>
         <v>0.22222222222222199</v>
       </c>
-      <c r="H9" s="187">
+      <c r="G9" s="187">
         <v>0.66666666666666696</v>
       </c>
-      <c r="I9" s="177">
-        <f>H10</f>
+      <c r="H9" s="176">
+        <f>G10</f>
         <v>0.33333333333333298</v>
       </c>
-      <c r="J9" s="176"/>
-      <c r="K9" s="176"/>
-    </row>
-    <row r="10" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="175"/>
+      <c r="J9" s="175"/>
+    </row>
+    <row r="10" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
-      <c r="D10" s="175" t="s">
+      <c r="D10" s="174" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="188">
+      <c r="E10" s="187">
         <v>0.22222222222222199</v>
       </c>
-      <c r="F10" s="176"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="187">
+      <c r="F10" s="2"/>
+      <c r="G10" s="187">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="176"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="11"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="175"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
         <v>177</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E12" s="187">
+      <c r="E12" s="257">
         <v>0.79166666666666696</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="176">
+      <c r="F12" s="175">
         <f>E13</f>
         <v>0.20833333333333301</v>
       </c>
-      <c r="H12" s="187">
+      <c r="G12" s="187">
         <v>0.66666700000000001</v>
       </c>
-      <c r="I12" s="177">
-        <f>H13</f>
+      <c r="H12" s="176">
+        <f>G13</f>
         <v>0.33333000000000002</v>
       </c>
-      <c r="J12" s="176"/>
-      <c r="K12" s="176"/>
-    </row>
-    <row r="13" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="175"/>
+      <c r="J12" s="175"/>
+    </row>
+    <row r="13" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="55"/>
       <c r="D13" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="E13" s="187">
+      <c r="E13" s="257">
         <v>0.20833333333333301</v>
       </c>
       <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="187">
+      <c r="G13" s="187">
         <v>0.33333000000000002</v>
       </c>
-      <c r="I13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="3:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="C15" s="181"/>
-      <c r="D15" s="184" t="s">
+    </row>
+    <row r="14" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="3:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="C15" s="180"/>
+      <c r="D15" s="183" t="s">
         <v>175</v>
       </c>
-      <c r="E15" s="184" t="s">
+      <c r="E15" s="183" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="183" t="s">
         <v>211</v>
       </c>
-      <c r="F15" s="184" t="s">
-        <v>212</v>
-      </c>
-      <c r="G15" s="184" t="s">
+      <c r="G15" s="183" t="s">
         <v>178</v>
       </c>
-      <c r="H15" s="184" t="s">
+      <c r="H15" s="183" t="s">
+        <v>192</v>
+      </c>
+      <c r="I15" s="198" t="s">
         <v>193</v>
       </c>
-      <c r="I15" s="200" t="s">
-        <v>194</v>
-      </c>
-      <c r="J15" s="184" t="s">
+      <c r="J15" s="183" t="s">
+        <v>188</v>
+      </c>
+      <c r="K15" s="183" t="s">
         <v>189</v>
       </c>
-      <c r="K15" s="184" t="s">
+      <c r="L15" s="183" t="s">
         <v>190</v>
       </c>
-      <c r="L15" s="184" t="s">
+      <c r="M15" s="181" t="s">
         <v>191</v>
       </c>
-      <c r="M15" s="182" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="16" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="185"/>
-      <c r="D16" s="183" t="s">
+    </row>
+    <row r="16" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="184"/>
+      <c r="D16" s="182" t="s">
         <v>176</v>
       </c>
-      <c r="E16" s="189"/>
-      <c r="F16" s="189"/>
-      <c r="G16" s="189" t="s">
+      <c r="E16" s="188"/>
+      <c r="F16" s="188"/>
+      <c r="G16" s="182" t="s">
         <v>162</v>
       </c>
-      <c r="H16" s="189" t="s">
+      <c r="H16" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="I16" s="201" t="s">
+      <c r="I16" s="199" t="s">
         <v>162</v>
       </c>
-      <c r="J16" s="189"/>
-      <c r="K16" s="189"/>
-      <c r="L16" s="189"/>
-      <c r="M16" s="190"/>
-    </row>
-    <row r="17" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="188"/>
+      <c r="K16" s="188"/>
+      <c r="L16" s="188"/>
+      <c r="M16" s="189"/>
+    </row>
+    <row r="17" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="187">
+      <c r="D17" s="186">
         <v>105800</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="199">
-        <v>354</v>
-      </c>
-      <c r="H17" s="176">
+      <c r="G17" s="186">
+        <v>458</v>
+      </c>
+      <c r="H17" s="175">
         <f>G17*'Applicance split'!G25</f>
-        <v>294.50060459492141</v>
-      </c>
-      <c r="I17" s="202">
+        <v>381.02055622732769</v>
+      </c>
+      <c r="I17" s="273">
         <f>G17*'Applicance split'!G24</f>
-        <v>59.499395405078594</v>
+        <v>76.979443772672298</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="187">
+      <c r="D18" s="186">
         <v>20000</v>
       </c>
-      <c r="E18" s="176">
-        <f>D18*G4/(D18*G4+D19*G9)</f>
+      <c r="E18" s="175">
+        <f>D18*F4/(D18*F4+D19*F9)</f>
         <v>0.27202753644137617</v>
       </c>
-      <c r="F18" s="176">
-        <f>D18*I4/(D18*I4+D19*I9)</f>
+      <c r="F18" s="175">
+        <f>D18*H4/(D18*H4+D19*H9)</f>
         <v>0.29298663248489282</v>
       </c>
-      <c r="G18" s="179"/>
-      <c r="H18" s="179">
+      <c r="G18" s="178"/>
+      <c r="H18" s="178">
         <f>H17*$E18</f>
-        <v>80.112273948452298</v>
-      </c>
-      <c r="I18" s="203">
+        <v>103.64808324404279</v>
+      </c>
+      <c r="I18" s="201">
         <f>I17*$F18</f>
-        <v>17.432527494621084</v>
-      </c>
-      <c r="J18" s="286">
-        <f>D28*H18</f>
-        <v>39.308059713247388</v>
-      </c>
-      <c r="K18" s="285">
-        <f>H18*E28</f>
-        <v>40.80421423520491</v>
-      </c>
-      <c r="L18" s="286">
-        <f>I18*D33</f>
-        <v>6.9730109978484336</v>
-      </c>
-      <c r="M18" s="286">
-        <f>I18*E33</f>
-        <v>10.459516496772652</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
+        <v>22.553948001515408</v>
+      </c>
+      <c r="J18" s="266">
+        <f>D26*H18</f>
+        <v>50.856190250472608</v>
+      </c>
+      <c r="K18" s="266">
+        <f>H18*E26</f>
+        <v>52.791892993570187</v>
+      </c>
+      <c r="L18" s="266">
+        <f>I18*D28</f>
+        <v>9.0215792006061637</v>
+      </c>
+      <c r="M18" s="272">
+        <f>I18*E28</f>
+        <v>13.532368800909246</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="10" t="s">
         <v>174</v>
       </c>
@@ -7992,344 +7958,202 @@
         <f>D17-D18</f>
         <v>85800</v>
       </c>
-      <c r="E19" s="176">
-        <f>D19*G9/(D18*G4+D19*G9)</f>
+      <c r="E19" s="175">
+        <f>D19*F9/(D18*F4+D19*F9)</f>
         <v>0.72797246355862388</v>
       </c>
-      <c r="F19" s="176">
-        <f>D19*I9/(D18*I4+D19*I9)</f>
+      <c r="F19" s="175">
+        <f>D19*H9/(D18*H4+D19*H9)</f>
         <v>0.70701336751510713</v>
       </c>
-      <c r="G19" s="179"/>
-      <c r="H19" s="179">
+      <c r="G19" s="178"/>
+      <c r="H19" s="178">
         <f>E19*$H17</f>
-        <v>214.38833064646914</v>
-      </c>
-      <c r="I19" s="203">
+        <v>277.37247298328492</v>
+      </c>
+      <c r="I19" s="201">
         <f>F19*$I17</f>
-        <v>42.066867910457511</v>
-      </c>
-      <c r="J19" s="214">
+        <v>54.425495771156882</v>
+      </c>
+      <c r="J19" s="266">
         <f>H19</f>
-        <v>214.38833064646914</v>
-      </c>
-      <c r="K19" s="214"/>
-      <c r="L19" s="214">
+        <v>277.37247298328492</v>
+      </c>
+      <c r="K19" s="266"/>
+      <c r="L19" s="266">
         <f>I19</f>
-        <v>42.066867910457511</v>
-      </c>
-      <c r="M19" s="215"/>
-    </row>
-    <row r="20" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>54.425495771156882</v>
+      </c>
+      <c r="M19" s="176"/>
+    </row>
+    <row r="20" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176"/>
+      <c r="H20" s="175"/>
+      <c r="I20" s="200"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="55" t="s">
         <v>177</v>
       </c>
-      <c r="D21" s="187">
+      <c r="D21" s="186">
         <v>37625</v>
       </c>
       <c r="E21" s="56"/>
       <c r="F21" s="56"/>
-      <c r="G21" s="187">
-        <v>458</v>
-      </c>
-      <c r="H21" s="196">
+      <c r="G21" s="186">
+        <v>354</v>
+      </c>
+      <c r="H21" s="195">
         <f>G21*'Applicance split'!G25</f>
-        <v>381.02055622732769</v>
-      </c>
-      <c r="I21" s="204">
+        <v>294.50060459492141</v>
+      </c>
+      <c r="I21" s="202">
         <f>G21*'Applicance split'!G24</f>
-        <v>76.979443772672298</v>
-      </c>
-      <c r="J21" s="180">
-        <f>H21/G12*E13</f>
-        <v>381.02055622732769</v>
-      </c>
-      <c r="K21" s="180"/>
-      <c r="L21" s="180">
-        <f>I21/I12*H13</f>
-        <v>76.979443772672298</v>
+        <v>59.499395405078594</v>
+      </c>
+      <c r="J21" s="179">
+        <f>H21/F12*E13</f>
+        <v>294.50060459492141</v>
+      </c>
+      <c r="K21" s="179"/>
+      <c r="L21" s="179">
+        <f>I21/H12*G13</f>
+        <v>59.499395405078594</v>
       </c>
       <c r="M21" s="105"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="J22" s="217">
-        <f>J18/SUM(J18:K18)</f>
-        <v>0.49066213921901525</v>
-      </c>
-      <c r="K22" s="217">
-        <f>K18/SUM(J18:K18)</f>
-        <v>0.50933786078098475</v>
-      </c>
-      <c r="L22" s="217">
-        <f>L18/SUM(L18:M18)</f>
-        <v>0.4</v>
-      </c>
-      <c r="M22" s="217">
-        <f>M18/SUM(L18:M18)</f>
-        <v>0.60000000000000009</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D24" s="3">
-        <f>E5*4.5</f>
-        <v>0.81255857544517507</v>
-      </c>
-      <c r="E24" s="3">
-        <f>1-D24</f>
-        <v>0.18744142455482493</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="D25" s="260" t="s">
-        <v>214</v>
-      </c>
-      <c r="E25" s="260" t="s">
+    <row r="22" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="213"/>
+      <c r="K22" s="213"/>
+      <c r="L22" s="213"/>
+      <c r="M22" s="213"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C23" s="291" t="s">
+        <v>248</v>
+      </c>
+      <c r="D23" s="292"/>
+      <c r="E23" s="293"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C24" s="268"/>
+      <c r="D24" s="267" t="s">
         <v>213</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="E24" s="269" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C25" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="J25" s="3">
-        <v>63.2</v>
-      </c>
-      <c r="K25" s="3">
-        <f>H4</f>
-        <v>0.44444444444444497</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C26" s="3" t="s">
-        <v>252</v>
-      </c>
       <c r="D26" s="262">
-        <f>1-E26</f>
-        <v>0.7999999999999996</v>
-      </c>
-      <c r="E26" s="262">
-        <f>E7*E6</f>
-        <v>0.2000000000000004</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="J26" s="3">
-        <v>18.059999999999999</v>
-      </c>
-      <c r="K26" s="3">
-        <f>H5</f>
-        <v>0.22222222222222199</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C27" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D27" s="3">
-        <f>D26/((E4+E5)/E5)</f>
-        <v>0.17777777777777792</v>
-      </c>
-      <c r="E27" s="3">
-        <f>E26/(E7)</f>
-        <v>0.18744142455482701</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="J27" s="3">
-        <v>18.739999999999998</v>
-      </c>
-      <c r="K27" s="3">
-        <f>H6</f>
-        <v>0.33333333333333298</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C28" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="D28" s="3">
         <f>E5/SUM(E5:E6)</f>
         <v>0.49066213921901525</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E26" s="265">
         <f>E6/SUM(E5:E6)</f>
         <v>0.50933786078098475</v>
       </c>
-      <c r="J28" s="3">
-        <v>1.0669999999999999</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="C29" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="I29" s="258" t="s">
-        <v>249</v>
-      </c>
-      <c r="J29" s="259">
-        <v>1.0125999999999999</v>
-      </c>
-      <c r="K29" s="259">
-        <v>0.9667</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="D30" s="260" t="s">
-        <v>214</v>
-      </c>
-      <c r="E30" s="260" t="s">
-        <v>213</v>
-      </c>
-      <c r="O30" s="186" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C31" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D31" s="262">
-        <f>1-E31</f>
-        <v>0.70000000000000029</v>
-      </c>
-      <c r="E31" s="262">
-        <f>H7*H6</f>
-        <v>0.29999999999999971</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C32" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D32" s="3">
-        <f>D31/((H4+H5)/H5)</f>
-        <v>0.23333333333333309</v>
-      </c>
-      <c r="E32" s="3">
-        <f>E31/(H7)</f>
-        <v>0.33333333333333298</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D33" s="283">
-        <f>H5/SUM(H5:H6)</f>
+    </row>
+    <row r="27" spans="3:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="C27" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" s="262"/>
+      <c r="E27" s="265"/>
+      <c r="I27" s="254"/>
+      <c r="J27" s="255"/>
+      <c r="K27" s="255"/>
+    </row>
+    <row r="28" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="D28" s="270">
+        <f>G5/SUM(G5:G6)</f>
         <v>0.4</v>
       </c>
-      <c r="E33" s="283">
-        <f>H6/SUM(H5:H6)</f>
+      <c r="E28" s="271">
+        <f>G6/SUM(G5:G6)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="J33" s="3">
-        <f>J27*J28</f>
-        <v>19.995579999999997</v>
-      </c>
-      <c r="K33" s="3">
-        <f>K27*K28</f>
-        <v>0.29999999999999971</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I35" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="J35" s="3">
-        <f>J33+J26+J25</f>
-        <v>101.25557999999999</v>
-      </c>
-      <c r="K35" s="3">
-        <f>K33+K26+K25</f>
-        <v>0.96666666666666667</v>
-      </c>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D38" s="261">
-        <f>E5*(SUM(E4:E5)/E5)</f>
-        <v>0.81255857544517396</v>
-      </c>
-      <c r="E38" s="261">
-        <f>H5*3</f>
-        <v>0.66666666666666596</v>
-      </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="261">
-        <f>E6*E7</f>
-        <v>0.2000000000000004</v>
-      </c>
-      <c r="E39" s="261">
-        <f>H6*0.9</f>
-        <v>0.29999999999999971</v>
-      </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="3">
-        <f>D38/SUM(D$38:D$39)</f>
-        <v>0.80248056275453505</v>
-      </c>
-      <c r="E41" s="3">
-        <f>E38/SUM(E$38:E$39)</f>
-        <v>0.68965517241379304</v>
-      </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D42" s="3">
-        <f>D39/SUM(D$38:D$39)</f>
-        <v>0.19751943724546484</v>
-      </c>
-      <c r="E42" s="3">
-        <f>E39/SUM(E$38:E$39)</f>
-        <v>0.31034482758620691</v>
-      </c>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D46" s="284">
-        <f>SUM(E4:E5)/E5</f>
-        <v>4.4999999999999938</v>
-      </c>
-      <c r="E46" s="284"/>
-      <c r="F46" s="284"/>
-      <c r="G46" s="293">
-        <f>SUM(H4:H5)/H5</f>
-        <v>3.0000000000000044</v>
-      </c>
-      <c r="H46" s="284"/>
+      <c r="H28" s="295"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H29" s="295"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H30" s="295"/>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H31" s="295"/>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H32" s="295"/>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D33" s="256"/>
+      <c r="E33" s="256"/>
+      <c r="H33" s="295"/>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D34" s="256"/>
+      <c r="E34" s="256"/>
+      <c r="H34" s="295"/>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="295"/>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="295"/>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="295"/>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="295"/>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="295"/>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H40" s="295"/>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D41" s="258"/>
+      <c r="E41" s="294"/>
+      <c r="F41" s="258"/>
+      <c r="G41" s="261"/>
+      <c r="H41" s="295"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:I2"/>
+  <mergeCells count="2">
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C2:H2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="O5" r:id="rId1"/>
-    <hyperlink ref="O30" r:id="rId2"/>
+    <hyperlink ref="N5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8351,7 +8175,7 @@
         <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
@@ -8364,7 +8188,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>